<commit_message>
fix: Update biometrics and survey import template Excel files
</commit_message>
<xml_diff>
--- a/docs/examples/biometrics_import_template.xlsx
+++ b/docs/examples/biometrics_import_template.xlsx
@@ -598,11 +598,6 @@
       <c r="G2" t="n">
         <v>100</v>
       </c>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr">
         <is>
           <t>ses-1</t>
@@ -628,7 +623,6 @@
           <t>Standard dynamometer protocol</t>
         </is>
       </c>
-      <c r="R2" t="inlineStr"/>
       <c r="S2" t="inlineStr">
         <is>
           <t>VORLAGENTEXT — bitte durch den finalen Instruktionstext ersetzen. Bitte beantworten Sie jede Frage ehrlich. Wählen Sie die Antwort aus, die am besten beschreibt, wie Sie sich in den letzten 7 Tagen gefühlt haben. Es gibt keine richtigen oder falschen Antworten.</t>
@@ -639,7 +633,6 @@
           <t>TEMPLATE TEXT — replace with your final participant wording. Please answer each question honestly. Select the option that best describes how you have felt during the last 7 days. There are no right or wrong answers.</t>
         </is>
       </c>
-      <c r="U2" t="inlineStr"/>
       <c r="V2" t="inlineStr">
         <is>
           <t>5 minutes</t>
@@ -655,8 +648,6 @@
           <t>investigator</t>
         </is>
       </c>
-      <c r="Y2" t="inlineStr"/>
-      <c r="Z2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -858,7 +849,6 @@
           <t>Semicolon-separated list of allowed values.</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -888,7 +878,6 @@
           <t>Alias of another variable.</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -952,7 +941,6 @@
           <t>Description of the study context.</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -982,7 +970,6 @@
           <t>General instructions.</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -995,7 +982,6 @@
           <t>Instructions in German.</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1008,7 +994,6 @@
           <t>Instructions in English.</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1021,7 +1006,6 @@
           <t>Reference or source for the procedure.</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">

</xml_diff>